<commit_message>
put code in folder R
</commit_message>
<xml_diff>
--- a/2022/data/status.xlsx
+++ b/2022/data/status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iattc-my.sharepoint.com/personal/hkxu_iattc_org/Documents/IATTC/2022/SAC13/Indicators/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iattc-my.sharepoint.com/personal/hkxu_iattc_org/Documents/Git/Indicators/2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABDACC10485439DF4C725BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAE40E89-9122-4F5F-AF78-5C13DC0F535B}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC10485439DF4C725BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BCD39D-F759-4ED9-A19E-9E55330E2EED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11055" yWindow="2205" windowWidth="17745" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update the DEL LF time series
</commit_message>
<xml_diff>
--- a/2022/data/status.xlsx
+++ b/2022/data/status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iattc-my.sharepoint.com/personal/hkxu_iattc_org/Documents/Git/Indicators/2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC10485439DF4C725BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BCD39D-F759-4ED9-A19E-9E55330E2EED}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_F25DC773A252ABDACC10485439DF4C725BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3636CF0A-8E29-4328-9DB4-C63D86F01F28}"/>
   <bookViews>
-    <workbookView xWindow="11055" yWindow="2205" windowWidth="17745" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -455,7 +455,7 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -479,7 +479,7 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>